<commit_message>
Trained "that was <flavor>" and "that was <bad/good>"
</commit_message>
<xml_diff>
--- a/training_info.xlsx
+++ b/training_info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t>drink</t>
   </si>
@@ -63,16 +63,19 @@
     <t>bad/good</t>
   </si>
   <si>
-    <t>trained</t>
-  </si>
-  <si>
     <t>able to train</t>
   </si>
   <si>
     <t>N/A?</t>
   </si>
   <si>
-    <t>bad? 1-257</t>
+    <t>training instances</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -114,94 +117,344 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -515,13 +768,13 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -538,10 +791,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -551,20 +804,20 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -574,17 +827,17 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>159</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -597,17 +850,17 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -620,17 +873,17 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -643,17 +896,17 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>79</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -666,17 +919,17 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>44</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -689,17 +942,17 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -712,14 +965,14 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="C9" t="s">
+        <v>18</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9">
-        <v>0</v>
+      <c r="E9" t="s">
+        <v>19</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -730,21 +983,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:G9">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"bad? 1-257"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"bad? 1-257"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:E9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Altered confirm_cushion, increased penalty for drinks, fixed confirmation
</commit_message>
<xml_diff>
--- a/training_info.xlsx
+++ b/training_info.xlsx
@@ -117,7 +117,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -125,306 +125,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -768,7 +468,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +629,7 @@
         <v>19</v>
       </c>
       <c r="F7">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -983,20 +683,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:G9">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"bad? 1-257"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"bad? 1-257"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>